<commit_message>
update at bt ct
</commit_message>
<xml_diff>
--- a/dataLatih/Book1.xlsx
+++ b/dataLatih/Book1.xlsx
@@ -641,11 +641,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="235130880"/>
-        <c:axId val="235132416"/>
+        <c:axId val="219139072"/>
+        <c:axId val="139780864"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="235130880"/>
+        <c:axId val="219139072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -688,7 +688,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="235132416"/>
+        <c:crossAx val="139780864"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -696,7 +696,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="235132416"/>
+        <c:axId val="139780864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -747,7 +747,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="235130880"/>
+        <c:crossAx val="219139072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1091,7 +1091,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1102,7 +1102,7 @@
   <dimension ref="A1:M31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1246,27 +1246,27 @@
         <v>16</v>
       </c>
       <c r="G4">
-        <f t="shared" ref="G4:G24" si="4">ROUND(0.1/2*(1-0.1)^2*((6-5*0.1)*C4-(10-8*0.1)*D4+(4-3*0.1)*E4),2)</f>
+        <f>ROUND(0.1/2*(1-0.1)^2*((6-5*0.1)*C4-(10-8*0.1)*D4+(4-3*0.1)*E4),2)</f>
         <v>0</v>
       </c>
       <c r="H4">
-        <f t="shared" ref="H4:H24" si="5">ROUND(0.1^2/(1-0.1)^2*(C4-2*D4+E4),2)</f>
+        <f t="shared" ref="H4:H24" si="4">ROUND(0.1^2/(1-0.1)^2*(C4-2*D4+E4),2)</f>
         <v>0</v>
       </c>
       <c r="I4" s="6">
-        <f t="shared" ref="I4:I23" si="6">ROUND(F4+G4*1+1/2*H4*1^2,0)</f>
+        <f t="shared" ref="I4:I23" si="5">ROUND(F4+G4*1+1/2*H4*1^2,0)</f>
         <v>16</v>
       </c>
       <c r="J4">
-        <f t="shared" ref="J4:J23" si="7">B4-I4</f>
+        <f t="shared" ref="J4:J23" si="6">B4-I4</f>
         <v>-1</v>
       </c>
       <c r="K4">
-        <f t="shared" ref="K4:K23" si="8">ABS(B4-I4)</f>
+        <f t="shared" ref="K4:K23" si="7">ABS(B4-I4)</f>
         <v>1</v>
       </c>
       <c r="L4">
-        <f t="shared" ref="L4:L23" si="9">J4^2</f>
+        <f t="shared" ref="L4:L23" si="8">J4^2</f>
         <v>1</v>
       </c>
       <c r="M4">
@@ -1306,23 +1306,23 @@
         <v>0</v>
       </c>
       <c r="I5" s="6">
+        <f t="shared" si="5"/>
+        <v>16</v>
+      </c>
+      <c r="J5">
         <f t="shared" si="6"/>
-        <v>16</v>
-      </c>
-      <c r="J5">
+        <v>6</v>
+      </c>
+      <c r="K5">
         <f t="shared" si="7"/>
         <v>6</v>
       </c>
-      <c r="K5">
+      <c r="L5">
         <f t="shared" si="8"/>
-        <v>6</v>
-      </c>
-      <c r="L5">
-        <f t="shared" si="9"/>
         <v>36</v>
       </c>
       <c r="M5">
-        <f t="shared" ref="M5:M23" si="10">ABS((B5-I5)/B5)</f>
+        <f t="shared" ref="M5:M23" si="9">ABS((B5-I5)/B5)</f>
         <v>0.27272727272727271</v>
       </c>
     </row>
@@ -1350,31 +1350,31 @@
         <v>17.41</v>
       </c>
       <c r="G6">
+        <f t="shared" ref="G4:G24" si="10">ROUND(0.1/2*(1-0.1)^2*((6-5*0.1)*C6-(10-8*0.1)*D6+(4-3*0.1)*E6),2)</f>
+        <v>0.1</v>
+      </c>
+      <c r="H6">
         <f t="shared" si="4"/>
-        <v>0.1</v>
-      </c>
-      <c r="H6">
+        <v>0.01</v>
+      </c>
+      <c r="I6" s="6">
         <f t="shared" si="5"/>
-        <v>0.01</v>
-      </c>
-      <c r="I6" s="6">
+        <v>18</v>
+      </c>
+      <c r="J6">
         <f t="shared" si="6"/>
-        <v>18</v>
-      </c>
-      <c r="J6">
+        <v>-10</v>
+      </c>
+      <c r="K6">
         <f t="shared" si="7"/>
-        <v>-10</v>
-      </c>
-      <c r="K6">
+        <v>10</v>
+      </c>
+      <c r="L6">
         <f t="shared" si="8"/>
-        <v>10</v>
-      </c>
-      <c r="L6">
+        <v>100</v>
+      </c>
+      <c r="M6">
         <f t="shared" si="9"/>
-        <v>100</v>
-      </c>
-      <c r="M6">
-        <f t="shared" si="10"/>
         <v>1.25</v>
       </c>
     </row>
@@ -1402,31 +1402,31 @@
         <v>14.98</v>
       </c>
       <c r="G7">
+        <f t="shared" si="10"/>
+        <v>-0.08</v>
+      </c>
+      <c r="H7">
         <f t="shared" si="4"/>
-        <v>-0.08</v>
-      </c>
-      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7" s="6">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="I7" s="6">
+        <v>15</v>
+      </c>
+      <c r="J7">
         <f t="shared" si="6"/>
-        <v>15</v>
-      </c>
-      <c r="J7">
+        <v>11</v>
+      </c>
+      <c r="K7">
         <f t="shared" si="7"/>
         <v>11</v>
       </c>
-      <c r="K7">
+      <c r="L7">
         <f t="shared" si="8"/>
-        <v>11</v>
-      </c>
-      <c r="L7">
+        <v>121</v>
+      </c>
+      <c r="M7">
         <f t="shared" si="9"/>
-        <v>121</v>
-      </c>
-      <c r="M7">
-        <f t="shared" si="10"/>
         <v>0.42307692307692307</v>
       </c>
     </row>
@@ -1454,31 +1454,31 @@
         <v>17.87</v>
       </c>
       <c r="G8">
+        <f t="shared" si="10"/>
+        <v>0.13</v>
+      </c>
+      <c r="H8">
         <f t="shared" si="4"/>
-        <v>0.13</v>
-      </c>
-      <c r="H8">
+        <v>0.01</v>
+      </c>
+      <c r="I8" s="6">
         <f t="shared" si="5"/>
-        <v>0.01</v>
-      </c>
-      <c r="I8" s="6">
+        <v>18</v>
+      </c>
+      <c r="J8">
         <f t="shared" si="6"/>
-        <v>18</v>
-      </c>
-      <c r="J8">
+        <v>-1</v>
+      </c>
+      <c r="K8">
         <f t="shared" si="7"/>
-        <v>-1</v>
-      </c>
-      <c r="K8">
+        <v>1</v>
+      </c>
+      <c r="L8">
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="L8">
+      <c r="M8">
         <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="M8">
-        <f t="shared" si="10"/>
         <v>5.8823529411764705E-2</v>
       </c>
     </row>
@@ -1506,31 +1506,31 @@
         <v>17.760000000000002</v>
       </c>
       <c r="G9">
+        <f t="shared" si="10"/>
+        <v>0.11</v>
+      </c>
+      <c r="H9">
         <f t="shared" si="4"/>
-        <v>0.11</v>
-      </c>
-      <c r="H9">
+        <v>0.01</v>
+      </c>
+      <c r="I9" s="6">
         <f t="shared" si="5"/>
-        <v>0.01</v>
-      </c>
-      <c r="I9" s="6">
+        <v>18</v>
+      </c>
+      <c r="J9">
         <f t="shared" si="6"/>
-        <v>18</v>
-      </c>
-      <c r="J9">
+        <v>24</v>
+      </c>
+      <c r="K9">
         <f t="shared" si="7"/>
         <v>24</v>
       </c>
-      <c r="K9">
+      <c r="L9">
         <f t="shared" si="8"/>
-        <v>24</v>
-      </c>
-      <c r="L9">
+        <v>576</v>
+      </c>
+      <c r="M9">
         <f t="shared" si="9"/>
-        <v>576</v>
-      </c>
-      <c r="M9">
-        <f t="shared" si="10"/>
         <v>0.5714285714285714</v>
       </c>
     </row>
@@ -1558,31 +1558,31 @@
         <v>24.46</v>
       </c>
       <c r="G10">
+        <f t="shared" si="10"/>
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="H10">
         <f t="shared" si="4"/>
-        <v>0.56999999999999995</v>
-      </c>
-      <c r="H10">
+        <v>0.03</v>
+      </c>
+      <c r="I10" s="6">
         <f t="shared" si="5"/>
-        <v>0.03</v>
-      </c>
-      <c r="I10" s="6">
+        <v>25</v>
+      </c>
+      <c r="J10">
         <f t="shared" si="6"/>
-        <v>25</v>
-      </c>
-      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="K10">
+      <c r="L10">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="L10">
+      <c r="M10">
         <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="M10">
-        <f t="shared" si="10"/>
         <v>0</v>
       </c>
     </row>
@@ -1610,31 +1610,31 @@
         <v>25.25</v>
       </c>
       <c r="G11">
+        <f t="shared" si="10"/>
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="H11">
         <f t="shared" si="4"/>
-        <v>0.57999999999999996</v>
-      </c>
-      <c r="H11">
+        <v>0.03</v>
+      </c>
+      <c r="I11" s="6">
         <f t="shared" si="5"/>
-        <v>0.03</v>
-      </c>
-      <c r="I11" s="6">
+        <v>26</v>
+      </c>
+      <c r="J11">
         <f t="shared" si="6"/>
-        <v>26</v>
-      </c>
-      <c r="J11">
+        <v>14</v>
+      </c>
+      <c r="K11">
         <f t="shared" si="7"/>
         <v>14</v>
       </c>
-      <c r="K11">
+      <c r="L11">
         <f t="shared" si="8"/>
-        <v>14</v>
-      </c>
-      <c r="L11">
+        <v>196</v>
+      </c>
+      <c r="M11">
         <f t="shared" si="9"/>
-        <v>196</v>
-      </c>
-      <c r="M11">
-        <f t="shared" si="10"/>
         <v>0.35</v>
       </c>
     </row>
@@ -1662,31 +1662,31 @@
         <v>29.9</v>
       </c>
       <c r="G12">
+        <f t="shared" si="10"/>
+        <v>0.86</v>
+      </c>
+      <c r="H12">
         <f t="shared" si="4"/>
-        <v>0.86</v>
-      </c>
-      <c r="H12">
+        <v>0.04</v>
+      </c>
+      <c r="I12" s="6">
         <f t="shared" si="5"/>
-        <v>0.04</v>
-      </c>
-      <c r="I12" s="6">
+        <v>31</v>
+      </c>
+      <c r="J12">
         <f t="shared" si="6"/>
-        <v>31</v>
-      </c>
-      <c r="J12">
+        <v>16</v>
+      </c>
+      <c r="K12">
         <f t="shared" si="7"/>
         <v>16</v>
       </c>
-      <c r="K12">
+      <c r="L12">
         <f t="shared" si="8"/>
-        <v>16</v>
-      </c>
-      <c r="L12">
+        <v>256</v>
+      </c>
+      <c r="M12">
         <f t="shared" si="9"/>
-        <v>256</v>
-      </c>
-      <c r="M12">
-        <f t="shared" si="10"/>
         <v>0.34042553191489361</v>
       </c>
     </row>
@@ -1714,31 +1714,31 @@
         <v>35.51</v>
       </c>
       <c r="G13">
+        <f t="shared" si="10"/>
+        <v>1.18</v>
+      </c>
+      <c r="H13">
         <f t="shared" si="4"/>
-        <v>1.18</v>
-      </c>
-      <c r="H13">
+        <v>0.06</v>
+      </c>
+      <c r="I13" s="6">
         <f t="shared" si="5"/>
-        <v>0.06</v>
-      </c>
-      <c r="I13" s="6">
+        <v>37</v>
+      </c>
+      <c r="J13">
         <f t="shared" si="6"/>
-        <v>37</v>
-      </c>
-      <c r="J13">
+        <v>10</v>
+      </c>
+      <c r="K13">
         <f t="shared" si="7"/>
         <v>10</v>
       </c>
-      <c r="K13">
+      <c r="L13">
         <f t="shared" si="8"/>
-        <v>10</v>
-      </c>
-      <c r="L13">
+        <v>100</v>
+      </c>
+      <c r="M13">
         <f t="shared" si="9"/>
-        <v>100</v>
-      </c>
-      <c r="M13">
-        <f t="shared" si="10"/>
         <v>0.21276595744680851</v>
       </c>
     </row>
@@ -1766,31 +1766,31 @@
         <v>39.950000000000003</v>
       </c>
       <c r="G14">
+        <f t="shared" si="10"/>
+        <v>1.4</v>
+      </c>
+      <c r="H14">
         <f t="shared" si="4"/>
-        <v>1.4</v>
-      </c>
-      <c r="H14">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="I14" s="6">
         <f t="shared" si="5"/>
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="I14" s="6">
+        <v>41</v>
+      </c>
+      <c r="J14">
         <f t="shared" si="6"/>
-        <v>41</v>
-      </c>
-      <c r="J14">
+        <v>-32</v>
+      </c>
+      <c r="K14">
         <f t="shared" si="7"/>
-        <v>-32</v>
-      </c>
-      <c r="K14">
+        <v>32</v>
+      </c>
+      <c r="L14">
         <f t="shared" si="8"/>
-        <v>32</v>
-      </c>
-      <c r="L14">
+        <v>1024</v>
+      </c>
+      <c r="M14">
         <f t="shared" si="9"/>
-        <v>1024</v>
-      </c>
-      <c r="M14">
-        <f t="shared" si="10"/>
         <v>3.5555555555555554</v>
       </c>
     </row>
@@ -1818,31 +1818,31 @@
         <v>33.15</v>
       </c>
       <c r="G15">
+        <f t="shared" si="10"/>
+        <v>0.83</v>
+      </c>
+      <c r="H15">
         <f t="shared" si="4"/>
-        <v>0.83</v>
-      </c>
-      <c r="H15">
+        <v>0.04</v>
+      </c>
+      <c r="I15" s="6">
         <f t="shared" si="5"/>
-        <v>0.04</v>
-      </c>
-      <c r="I15" s="6">
+        <v>34</v>
+      </c>
+      <c r="J15">
         <f t="shared" si="6"/>
-        <v>34</v>
-      </c>
-      <c r="J15">
+        <v>-5</v>
+      </c>
+      <c r="K15">
         <f t="shared" si="7"/>
-        <v>-5</v>
-      </c>
-      <c r="K15">
+        <v>5</v>
+      </c>
+      <c r="L15">
         <f t="shared" si="8"/>
-        <v>5</v>
-      </c>
-      <c r="L15">
+        <v>25</v>
+      </c>
+      <c r="M15">
         <f t="shared" si="9"/>
-        <v>25</v>
-      </c>
-      <c r="M15">
-        <f t="shared" si="10"/>
         <v>0.17241379310344829</v>
       </c>
     </row>
@@ -1870,31 +1870,31 @@
         <v>32.950000000000003</v>
       </c>
       <c r="G16">
+        <f t="shared" si="10"/>
+        <v>0.75</v>
+      </c>
+      <c r="H16">
         <f t="shared" si="4"/>
-        <v>0.75</v>
-      </c>
-      <c r="H16">
+        <v>0.03</v>
+      </c>
+      <c r="I16" s="6">
         <f t="shared" si="5"/>
-        <v>0.03</v>
-      </c>
-      <c r="I16" s="6">
+        <v>34</v>
+      </c>
+      <c r="J16">
         <f t="shared" si="6"/>
-        <v>34</v>
-      </c>
-      <c r="J16">
+        <v>-14</v>
+      </c>
+      <c r="K16">
         <f t="shared" si="7"/>
-        <v>-14</v>
-      </c>
-      <c r="K16">
+        <v>14</v>
+      </c>
+      <c r="L16">
         <f t="shared" si="8"/>
-        <v>14</v>
-      </c>
-      <c r="L16">
+        <v>196</v>
+      </c>
+      <c r="M16">
         <f t="shared" si="9"/>
-        <v>196</v>
-      </c>
-      <c r="M16">
-        <f t="shared" si="10"/>
         <v>0.7</v>
       </c>
     </row>
@@ -1922,31 +1922,31 @@
         <v>30.28</v>
       </c>
       <c r="G17">
+        <f t="shared" si="10"/>
+        <v>0.5</v>
+      </c>
+      <c r="H17">
         <f t="shared" si="4"/>
-        <v>0.5</v>
-      </c>
-      <c r="H17">
+        <v>0.02</v>
+      </c>
+      <c r="I17" s="6">
         <f t="shared" si="5"/>
-        <v>0.02</v>
-      </c>
-      <c r="I17" s="6">
+        <v>31</v>
+      </c>
+      <c r="J17">
         <f t="shared" si="6"/>
-        <v>31</v>
-      </c>
-      <c r="J17">
+        <v>-9</v>
+      </c>
+      <c r="K17">
         <f t="shared" si="7"/>
-        <v>-9</v>
-      </c>
-      <c r="K17">
+        <v>9</v>
+      </c>
+      <c r="L17">
         <f t="shared" si="8"/>
-        <v>9</v>
-      </c>
-      <c r="L17">
+        <v>81</v>
+      </c>
+      <c r="M17">
         <f t="shared" si="9"/>
-        <v>81</v>
-      </c>
-      <c r="M17">
-        <f t="shared" si="10"/>
         <v>0.40909090909090912</v>
       </c>
     </row>
@@ -1974,31 +1974,31 @@
         <v>28.6</v>
       </c>
       <c r="G18">
+        <f t="shared" si="10"/>
+        <v>0.34</v>
+      </c>
+      <c r="H18">
         <f t="shared" si="4"/>
-        <v>0.34</v>
-      </c>
-      <c r="H18">
+        <v>0.01</v>
+      </c>
+      <c r="I18" s="6">
         <f t="shared" si="5"/>
-        <v>0.01</v>
-      </c>
-      <c r="I18" s="6">
+        <v>29</v>
+      </c>
+      <c r="J18">
         <f t="shared" si="6"/>
-        <v>29</v>
-      </c>
-      <c r="J18">
+        <v>-12</v>
+      </c>
+      <c r="K18">
         <f t="shared" si="7"/>
-        <v>-12</v>
-      </c>
-      <c r="K18">
+        <v>12</v>
+      </c>
+      <c r="L18">
         <f t="shared" si="8"/>
-        <v>12</v>
-      </c>
-      <c r="L18">
+        <v>144</v>
+      </c>
+      <c r="M18">
         <f t="shared" si="9"/>
-        <v>144</v>
-      </c>
-      <c r="M18">
-        <f t="shared" si="10"/>
         <v>0.70588235294117652</v>
       </c>
     </row>
@@ -2026,31 +2026,31 @@
         <v>25.84</v>
       </c>
       <c r="G19">
+        <f t="shared" si="10"/>
+        <v>0.12</v>
+      </c>
+      <c r="H19">
         <f t="shared" si="4"/>
-        <v>0.12</v>
-      </c>
-      <c r="H19">
+        <v>-0.01</v>
+      </c>
+      <c r="I19" s="6">
         <f t="shared" si="5"/>
-        <v>-0.01</v>
-      </c>
-      <c r="I19" s="6">
+        <v>26</v>
+      </c>
+      <c r="J19">
         <f t="shared" si="6"/>
-        <v>26</v>
-      </c>
-      <c r="J19">
+        <v>-20</v>
+      </c>
+      <c r="K19">
         <f t="shared" si="7"/>
-        <v>-20</v>
-      </c>
-      <c r="K19">
+        <v>20</v>
+      </c>
+      <c r="L19">
         <f t="shared" si="8"/>
-        <v>20</v>
-      </c>
-      <c r="L19">
+        <v>400</v>
+      </c>
+      <c r="M19">
         <f t="shared" si="9"/>
-        <v>400</v>
-      </c>
-      <c r="M19">
-        <f t="shared" si="10"/>
         <v>3.3333333333333335</v>
       </c>
     </row>
@@ -2078,31 +2078,31 @@
         <v>20.59</v>
       </c>
       <c r="G20">
+        <f t="shared" si="10"/>
+        <v>-0.26</v>
+      </c>
+      <c r="H20">
         <f t="shared" si="4"/>
-        <v>-0.26</v>
-      </c>
-      <c r="H20">
+        <v>-0.03</v>
+      </c>
+      <c r="I20" s="6">
         <f t="shared" si="5"/>
-        <v>-0.03</v>
-      </c>
-      <c r="I20" s="6">
+        <v>20</v>
+      </c>
+      <c r="J20">
         <f t="shared" si="6"/>
-        <v>20</v>
-      </c>
-      <c r="J20">
+        <v>-4</v>
+      </c>
+      <c r="K20">
         <f t="shared" si="7"/>
-        <v>-4</v>
-      </c>
-      <c r="K20">
+        <v>4</v>
+      </c>
+      <c r="L20">
         <f t="shared" si="8"/>
-        <v>4</v>
-      </c>
-      <c r="L20">
+        <v>16</v>
+      </c>
+      <c r="M20">
         <f t="shared" si="9"/>
-        <v>16</v>
-      </c>
-      <c r="M20">
-        <f t="shared" si="10"/>
         <v>0.25</v>
       </c>
     </row>
@@ -2130,31 +2130,31 @@
         <v>19.03</v>
       </c>
       <c r="G21">
+        <f t="shared" si="10"/>
+        <v>-0.35</v>
+      </c>
+      <c r="H21">
         <f t="shared" si="4"/>
-        <v>-0.35</v>
-      </c>
-      <c r="H21">
+        <v>-0.03</v>
+      </c>
+      <c r="I21" s="6">
         <f t="shared" si="5"/>
-        <v>-0.03</v>
-      </c>
-      <c r="I21" s="6">
+        <v>19</v>
+      </c>
+      <c r="J21">
         <f t="shared" si="6"/>
-        <v>19</v>
-      </c>
-      <c r="J21">
+        <v>-7</v>
+      </c>
+      <c r="K21">
         <f t="shared" si="7"/>
-        <v>-7</v>
-      </c>
-      <c r="K21">
+        <v>7</v>
+      </c>
+      <c r="L21">
         <f t="shared" si="8"/>
-        <v>7</v>
-      </c>
-      <c r="L21">
+        <v>49</v>
+      </c>
+      <c r="M21">
         <f t="shared" si="9"/>
-        <v>49</v>
-      </c>
-      <c r="M21">
-        <f t="shared" si="10"/>
         <v>0.58333333333333337</v>
       </c>
     </row>
@@ -2182,31 +2182,31 @@
         <v>16.72</v>
       </c>
       <c r="G22">
+        <f t="shared" si="10"/>
+        <v>-0.49</v>
+      </c>
+      <c r="H22">
         <f t="shared" si="4"/>
-        <v>-0.49</v>
-      </c>
-      <c r="H22">
+        <v>-0.04</v>
+      </c>
+      <c r="I22" s="6">
         <f t="shared" si="5"/>
-        <v>-0.04</v>
-      </c>
-      <c r="I22" s="6">
+        <v>16</v>
+      </c>
+      <c r="J22">
         <f t="shared" si="6"/>
-        <v>16</v>
-      </c>
-      <c r="J22">
+        <v>-9</v>
+      </c>
+      <c r="K22">
         <f t="shared" si="7"/>
-        <v>-9</v>
-      </c>
-      <c r="K22">
+        <v>9</v>
+      </c>
+      <c r="L22">
         <f t="shared" si="8"/>
-        <v>9</v>
-      </c>
-      <c r="L22">
+        <v>81</v>
+      </c>
+      <c r="M22">
         <f t="shared" si="9"/>
-        <v>81</v>
-      </c>
-      <c r="M22">
-        <f t="shared" si="10"/>
         <v>1.2857142857142858</v>
       </c>
     </row>
@@ -2234,31 +2234,31 @@
         <v>13.52</v>
       </c>
       <c r="G23">
+        <f t="shared" si="10"/>
+        <v>-0.69</v>
+      </c>
+      <c r="H23">
         <f t="shared" si="4"/>
-        <v>-0.69</v>
-      </c>
-      <c r="H23">
+        <v>-0.05</v>
+      </c>
+      <c r="I23" s="6">
         <f t="shared" si="5"/>
-        <v>-0.05</v>
-      </c>
-      <c r="I23" s="6">
+        <v>13</v>
+      </c>
+      <c r="J23">
         <f t="shared" si="6"/>
-        <v>13</v>
-      </c>
-      <c r="J23">
+        <v>-6</v>
+      </c>
+      <c r="K23">
         <f t="shared" si="7"/>
-        <v>-6</v>
-      </c>
-      <c r="K23">
+        <v>6</v>
+      </c>
+      <c r="L23">
         <f t="shared" si="8"/>
-        <v>6</v>
-      </c>
-      <c r="L23">
+        <v>36</v>
+      </c>
+      <c r="M23">
         <f t="shared" si="9"/>
-        <v>36</v>
-      </c>
-      <c r="M23">
-        <f t="shared" si="10"/>
         <v>0.8571428571428571</v>
       </c>
     </row>
@@ -2284,11 +2284,11 @@
         <v>10.96</v>
       </c>
       <c r="G24" s="1">
+        <f t="shared" si="10"/>
+        <v>-0.82</v>
+      </c>
+      <c r="H24" s="1">
         <f t="shared" si="4"/>
-        <v>-0.82</v>
-      </c>
-      <c r="H24" s="1">
-        <f t="shared" si="5"/>
         <v>-0.05</v>
       </c>
       <c r="I24" s="5">

</xml_diff>